<commit_message>
Create Client Full Module
Completed

-With Photos and Signatures.

Used masking for ID formats
</commit_message>
<xml_diff>
--- a/public/OFFICE STRUCTURE.xlsx
+++ b/public/OFFICE STRUCTURE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashbeemorgado/devs/lumen/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26286322-467F-0A4A-9AFD-C4D5BF7FB820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11611B9-9E74-0549-98F9-358DB6B48A38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20560" xr2:uid="{B219841F-3218-4145-B920-CF973D62632C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20560" xr2:uid="{B219841F-3218-4145-B920-CF973D62632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A1E2B0-13DC-394E-86C0-419AFE350589}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,7 +995,7 @@
         <v>107</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>105</v>
@@ -1012,7 +1012,7 @@
         <v>108</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>104</v>
@@ -2650,14 +2650,6 @@
       <c r="E75" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F75" t="str">
-        <f t="shared" si="0"/>
-        <v>051PSY-A101-UNIT-A</v>
-      </c>
-      <c r="G75" t="str">
-        <f t="shared" si="1"/>
-        <v>051PSY-A101-UNIT-B</v>
-      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -2675,14 +2667,6 @@
       <c r="E76" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F76" t="str">
-        <f t="shared" si="0"/>
-        <v>051PSY-A102-UNIT-A</v>
-      </c>
-      <c r="G76" t="str">
-        <f t="shared" si="1"/>
-        <v>051PSY-A102-UNIT-B</v>
-      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -2700,14 +2684,6 @@
       <c r="E77" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F77" t="str">
-        <f t="shared" si="0"/>
-        <v>051PSY-A103-UNIT-A</v>
-      </c>
-      <c r="G77" t="str">
-        <f t="shared" si="1"/>
-        <v>051PSY-A103-UNIT-B</v>
-      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
@@ -2725,14 +2701,6 @@
       <c r="E78" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F78" t="str">
-        <f t="shared" si="0"/>
-        <v>051PSY-A104-UNIT-A</v>
-      </c>
-      <c r="G78" t="str">
-        <f t="shared" si="1"/>
-        <v>051PSY-A104-UNIT-B</v>
-      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
@@ -2749,14 +2717,6 @@
       </c>
       <c r="E79" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="F79" t="str">
-        <f t="shared" si="0"/>
-        <v>051PSY-AO-UNIT-A</v>
-      </c>
-      <c r="G79" t="str">
-        <f t="shared" si="1"/>
-        <v>051PSY-AO-UNIT-B</v>
       </c>
     </row>
   </sheetData>

</xml_diff>